<commit_message>
Updated, but we're still missing some points
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/tpk5401_psu_edu/Documents/Courses/AERSP_424/Spring 2024/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Luis\Documents\School\Aersp424\FINAL_PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="463" documentId="8_{2E687571-912A-48DF-A2AF-07FCC8CEC5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C01A4D37-18CA-4B03-AC58-B97C6393B3DA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A13C604-E49E-47AD-84FE-9E7A569626E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Checklist</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Concurrent Programming</t>
   </si>
   <si>
-    <t>Get full credit (30% of the final grade) if you score more than or equal to 30/50</t>
-  </si>
-  <si>
     <t>1 - The code is fairly easy to read, 0 - readable only by someone who knows what it is supposed to be doing, or the code is poorly organized and difficult to read.</t>
   </si>
   <si>
@@ -198,13 +195,70 @@
   </si>
   <si>
     <t>0 - single thread, 1 - two or more threads without resource sharing, 2 - Two or more threads with resource sharing, 2.5 - Two or more threads with resource sharing and no errors</t>
+  </si>
+  <si>
+    <t>Brainstorm Ideas</t>
+  </si>
+  <si>
+    <t>Multithreading: Have one thread that constantly checks if there are enough equations and known variables to solve for some unknown variables.</t>
+  </si>
+  <si>
+    <t>Include a lot of comments and be smart of how we name our variables</t>
+  </si>
+  <si>
+    <t>Include some equations from Aersp 309</t>
+  </si>
+  <si>
+    <t>Can represent multiple boolean states using a single bit- each bit represents a different variable. See this website.</t>
+  </si>
+  <si>
+    <t>Have pre-programmed rocket parts that you can choose from</t>
+  </si>
+  <si>
+    <t>Create a class that inherits properties of another one</t>
+  </si>
+  <si>
+    <t>Option to save the output to a .txt file</t>
+  </si>
+  <si>
+    <t>Overriding inhereted functions</t>
+  </si>
+  <si>
+    <t>Create a class for the whole rocket as well as each of the individual components</t>
+  </si>
+  <si>
+    <t>Create objects from a class</t>
+  </si>
+  <si>
+    <t>Look for bugs (e.g. recognize if the user tries to input a negative amount of fuel)</t>
+  </si>
+  <si>
+    <t>Create a library for all our functions</t>
+  </si>
+  <si>
+    <t>Create a library for all our functions. Create header files for all our functions</t>
+  </si>
+  <si>
+    <t>The rocket object accepts pointers of the sub-components. (e.g: using pointers, we can tell the rocket how many stages it has, what boosters it's using, etc.)</t>
+  </si>
+  <si>
+    <t>Create multiple functions that have different parameters.</t>
+  </si>
+  <si>
+    <t>Create a function</t>
+  </si>
+  <si>
+    <t>create if statements and for loops</t>
+  </si>
+  <si>
+    <t>Get full credit (30% of the final grade) if you score more than or equal to 30/35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,16 +289,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -252,19 +320,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -281,9 +377,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -321,7 +417,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -427,7 +523,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -569,7 +665,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -577,329 +673,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.28515625" customWidth="1"/>
+    <col min="5" max="5" width="168.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="6"/>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="6"/>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
       <c r="B11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12">
         <v>0.5</v>
       </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="6"/>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
       <c r="B22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
-      <c r="D23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="D24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="D25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="D26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="8"/>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="D28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29" s="6"/>
+      <c r="E29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C30" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>2.5</v>
       </c>
-      <c r="D32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -907,32 +1072,45 @@
         <f>SUM(B3:B32)</f>
         <v>35</v>
       </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="3"/>
+      <c r="D33">
+        <f>SUM(D3:D32)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C14" r:id="rId1" xr:uid="{E4863355-EAAB-4B96-A2C1-0136E775C375}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>